<commit_message>
excel of WGD results
</commit_message>
<xml_diff>
--- a/HiFi_assemblies/C_amplexicaulis_S_pinnata_comparisons/output/genespace_no_pinnata/WGD_retention_loss_GO.xlsx
+++ b/HiFi_assemblies/C_amplexicaulis_S_pinnata_comparisons/output/genespace_no_pinnata/WGD_retention_loss_GO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmaloof/git/Davis_Dimensions_Sdiv_Assembly/HiFi_assemblies/C_amplexicaulis_S_pinnata_comparisons/output/genespace_no_pinnata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C4F8CD76-F312-1741-839F-672A69541D21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E56E9FCE-45E3-764A-9A4E-2E541D845449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12400" yWindow="2600" windowWidth="26440" windowHeight="15440" xr2:uid="{8D8973C9-0276-D64F-9CDA-5047CB7ECE61}"/>
+    <workbookView xWindow="23780" yWindow="3040" windowWidth="16360" windowHeight="14140" xr2:uid="{8D8973C9-0276-D64F-9CDA-5047CB7ECE61}"/>
   </bookViews>
   <sheets>
     <sheet name="WGD_retention_loss_GO" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="56">
   <si>
     <t>Category</t>
   </si>
@@ -43,18 +43,12 @@
     <t>GO:0006355</t>
   </si>
   <si>
-    <t>regulation of DNA-templated transcriptio...</t>
-  </si>
-  <si>
     <t>GO:0006886</t>
   </si>
   <si>
     <t>intracellular protein transport</t>
   </si>
   <si>
-    <t>both lost</t>
-  </si>
-  <si>
     <t>GO:0005975</t>
   </si>
   <si>
@@ -148,9 +142,6 @@
     <t>GO:0042430</t>
   </si>
   <si>
-    <t>indole-containing compound metabolic pro...</t>
-  </si>
-  <si>
     <t>GO:0045132</t>
   </si>
   <si>
@@ -160,9 +151,6 @@
     <t>GO:0070192</t>
   </si>
   <si>
-    <t>chromosome organization involved in meio...</t>
-  </si>
-  <si>
     <t>GO:0006576</t>
   </si>
   <si>
@@ -179,13 +167,34 @@
   </si>
   <si>
     <t>n in Group</t>
+  </si>
+  <si>
+    <t>S_div. #</t>
+  </si>
+  <si>
+    <t>C_amp. #</t>
+  </si>
+  <si>
+    <t>1 or 0</t>
+  </si>
+  <si>
+    <t>both single</t>
+  </si>
+  <si>
+    <t>regulation of DNA-templated transcription</t>
+  </si>
+  <si>
+    <t>chromosome organization involved in meiosis</t>
+  </si>
+  <si>
+    <t>indole-containing compound metabolic process</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -326,6 +335,12 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -676,12 +691,21 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="11" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1057,526 +1081,661 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D75D7403-A256-4248-B6EA-CC1A4956221D}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.33203125" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" customWidth="1"/>
-    <col min="3" max="3" width="38.1640625" customWidth="1"/>
+    <col min="1" max="1" width="19.1640625" customWidth="1"/>
+    <col min="2" max="2" width="7.83203125" customWidth="1"/>
+    <col min="3" max="3" width="9.33203125" customWidth="1"/>
+    <col min="4" max="4" width="11.83203125" customWidth="1"/>
+    <col min="5" max="5" width="39" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>51</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>52</v>
+        <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6">
+        <v>2</v>
+      </c>
+      <c r="C2" s="6">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="3">
+      <c r="E2" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="3">
         <v>434</v>
       </c>
-      <c r="E2" s="3">
+      <c r="G2" s="3">
         <v>355</v>
       </c>
-      <c r="F2" s="3">
+      <c r="H2" s="3">
         <v>322.57</v>
       </c>
-      <c r="G2" s="3">
+      <c r="I2" s="3">
         <v>1.9000000000000001E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="6">
+        <v>2</v>
+      </c>
+      <c r="C3" s="6">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="F3" s="3">
+        <v>91</v>
+      </c>
+      <c r="G3" s="3">
+        <v>80</v>
+      </c>
+      <c r="H3" s="3">
+        <v>67.64</v>
+      </c>
+      <c r="I3" s="3">
+        <v>7.2999999999999996E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="7">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="3">
-        <v>91</v>
-      </c>
-      <c r="E3" s="3">
-        <v>80</v>
-      </c>
-      <c r="F3" s="3">
-        <v>67.64</v>
-      </c>
-      <c r="G3" s="3">
-        <v>7.2999999999999996E-4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="E4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="F4">
+        <v>257</v>
+      </c>
+      <c r="G4">
+        <v>37</v>
+      </c>
+      <c r="H4">
+        <v>19.29</v>
+      </c>
+      <c r="I4" s="1">
+        <v>1.8E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="7">
+        <v>1</v>
+      </c>
+      <c r="C5" s="7">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="E5" t="s">
         <v>12</v>
       </c>
-      <c r="D4">
-        <v>257</v>
-      </c>
-      <c r="E4">
+      <c r="F5">
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <v>3</v>
+      </c>
+      <c r="H5">
+        <v>0.38</v>
+      </c>
+      <c r="I5">
+        <v>5.5999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="7">
+        <v>1</v>
+      </c>
+      <c r="C6" s="7">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E6" t="s">
+        <v>14</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+      <c r="G6">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>0.15</v>
+      </c>
+      <c r="I6">
+        <v>5.5999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="7">
+        <v>1</v>
+      </c>
+      <c r="C7" s="7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7">
+        <v>188</v>
+      </c>
+      <c r="G7">
+        <v>21</v>
+      </c>
+      <c r="H7">
+        <v>14.11</v>
+      </c>
+      <c r="I7">
+        <v>7.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="6">
+        <v>2</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F8" s="3">
+        <v>5</v>
+      </c>
+      <c r="G8" s="3">
+        <v>4</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="I8" s="4">
+        <v>4.6E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="6">
+        <v>2</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="3">
+        <v>305</v>
+      </c>
+      <c r="G9" s="3">
+        <v>30</v>
+      </c>
+      <c r="H9" s="3">
+        <v>17.11</v>
+      </c>
+      <c r="I9" s="3">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="6">
+        <v>2</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="3">
+        <v>18</v>
+      </c>
+      <c r="G10" s="3">
+        <v>4</v>
+      </c>
+      <c r="H10" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="I10" s="3">
+        <v>3.0999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="7">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>25</v>
+      </c>
+      <c r="E11" t="s">
+        <v>26</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="G11">
+        <v>3</v>
+      </c>
+      <c r="H11">
+        <v>0.38</v>
+      </c>
+      <c r="I11">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="7">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12">
+        <v>3</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12">
+        <v>0.38</v>
+      </c>
+      <c r="I12">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C13" s="7">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13">
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+      <c r="H13">
+        <v>0.38</v>
+      </c>
+      <c r="I13">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="7">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>3</v>
+      </c>
+      <c r="H14">
+        <v>0.38</v>
+      </c>
+      <c r="I14">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C15" s="7">
+        <v>2</v>
+      </c>
+      <c r="D15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15">
+        <v>6</v>
+      </c>
+      <c r="G15">
+        <v>4</v>
+      </c>
+      <c r="H15">
+        <v>0.75</v>
+      </c>
+      <c r="I15">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C16" s="7">
+        <v>2</v>
+      </c>
+      <c r="D16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E16" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16">
+        <v>6</v>
+      </c>
+      <c r="G16">
+        <v>4</v>
+      </c>
+      <c r="H16">
+        <v>0.75</v>
+      </c>
+      <c r="I16">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C17" s="7">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
         <v>37</v>
       </c>
-      <c r="F4">
-        <v>19.29</v>
-      </c>
-      <c r="G4" s="1">
-        <v>1.8E-5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5">
+      <c r="E17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17">
+        <v>6</v>
+      </c>
+      <c r="G17">
+        <v>4</v>
+      </c>
+      <c r="H17">
+        <v>0.75</v>
+      </c>
+      <c r="I17">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" s="7">
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" t="s">
+        <v>55</v>
+      </c>
+      <c r="F18">
+        <v>6</v>
+      </c>
+      <c r="G18">
+        <v>4</v>
+      </c>
+      <c r="H18">
+        <v>0.75</v>
+      </c>
+      <c r="I18">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C19" s="7">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E19" t="s">
+        <v>41</v>
+      </c>
+      <c r="F19">
+        <v>4</v>
+      </c>
+      <c r="G19">
+        <v>3</v>
+      </c>
+      <c r="H19">
+        <v>0.5</v>
+      </c>
+      <c r="I19">
+        <v>7.1000000000000004E-3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C20" s="7">
+        <v>2</v>
+      </c>
+      <c r="D20" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" t="s">
+        <v>54</v>
+      </c>
+      <c r="F20">
+        <v>4</v>
+      </c>
+      <c r="G20">
+        <v>3</v>
+      </c>
+      <c r="H20">
+        <v>0.5</v>
+      </c>
+      <c r="I20">
+        <v>7.1000000000000004E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C21" s="7">
+        <v>2</v>
+      </c>
+      <c r="D21" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" t="s">
+        <v>44</v>
+      </c>
+      <c r="F21">
+        <v>11</v>
+      </c>
+      <c r="G21">
         <v>5</v>
       </c>
-      <c r="E5">
-        <v>3</v>
-      </c>
-      <c r="F5">
-        <v>0.38</v>
-      </c>
-      <c r="G5">
-        <v>5.5999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6">
-        <v>2</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6">
-        <v>0.15</v>
-      </c>
-      <c r="G6">
-        <v>5.5999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7">
-        <v>188</v>
-      </c>
-      <c r="E7">
+      <c r="H21">
+        <v>1.38</v>
+      </c>
+      <c r="I21">
+        <v>7.4000000000000003E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="C22" s="7">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22">
+        <v>99</v>
+      </c>
+      <c r="G22">
         <v>21</v>
       </c>
-      <c r="F7">
-        <v>14.11</v>
-      </c>
-      <c r="G7">
-        <v>7.4000000000000003E-3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="D8" s="3">
-        <v>5</v>
-      </c>
-      <c r="E8" s="3">
-        <v>4</v>
-      </c>
-      <c r="F8" s="3">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="G8" s="4">
-        <v>4.6E-5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D9" s="3">
-        <v>305</v>
-      </c>
-      <c r="E9" s="3">
-        <v>30</v>
-      </c>
-      <c r="F9" s="3">
-        <v>17.11</v>
-      </c>
-      <c r="G9" s="3">
-        <v>3.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D10" s="3">
-        <v>18</v>
-      </c>
-      <c r="E10" s="3">
-        <v>4</v>
-      </c>
-      <c r="F10" s="3">
-        <v>1.01</v>
-      </c>
-      <c r="G10" s="3">
-        <v>3.0999999999999999E-3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11">
-        <v>3</v>
-      </c>
-      <c r="E11">
-        <v>3</v>
-      </c>
-      <c r="F11">
-        <v>0.38</v>
-      </c>
-      <c r="G11">
-        <v>2E-3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12">
-        <v>3</v>
-      </c>
-      <c r="E12">
-        <v>3</v>
-      </c>
-      <c r="F12">
-        <v>0.38</v>
-      </c>
-      <c r="G12">
-        <v>2E-3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D13">
-        <v>3</v>
-      </c>
-      <c r="E13">
-        <v>3</v>
-      </c>
-      <c r="F13">
-        <v>0.38</v>
-      </c>
-      <c r="G13">
-        <v>2E-3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>26</v>
-      </c>
-      <c r="B14" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14">
-        <v>3</v>
-      </c>
-      <c r="E14">
-        <v>3</v>
-      </c>
-      <c r="F14">
-        <v>0.38</v>
-      </c>
-      <c r="G14">
-        <v>2E-3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>26</v>
-      </c>
-      <c r="B15" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15">
-        <v>6</v>
-      </c>
-      <c r="E15">
-        <v>4</v>
-      </c>
-      <c r="F15">
-        <v>0.75</v>
-      </c>
-      <c r="G15">
-        <v>3.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C16" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16">
-        <v>6</v>
-      </c>
-      <c r="E16">
-        <v>4</v>
-      </c>
-      <c r="F16">
-        <v>0.75</v>
-      </c>
-      <c r="G16">
-        <v>3.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" t="s">
-        <v>39</v>
-      </c>
-      <c r="C17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D17">
-        <v>6</v>
-      </c>
-      <c r="E17">
-        <v>4</v>
-      </c>
-      <c r="F17">
-        <v>0.75</v>
-      </c>
-      <c r="G17">
-        <v>3.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>26</v>
-      </c>
-      <c r="B18" t="s">
-        <v>41</v>
-      </c>
-      <c r="C18" t="s">
-        <v>42</v>
-      </c>
-      <c r="D18">
-        <v>6</v>
-      </c>
-      <c r="E18">
-        <v>4</v>
-      </c>
-      <c r="F18">
-        <v>0.75</v>
-      </c>
-      <c r="G18">
-        <v>3.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" t="s">
-        <v>44</v>
-      </c>
-      <c r="D19">
-        <v>4</v>
-      </c>
-      <c r="E19">
-        <v>3</v>
-      </c>
-      <c r="F19">
-        <v>0.5</v>
-      </c>
-      <c r="G19">
-        <v>7.1000000000000004E-3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B20" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" t="s">
-        <v>46</v>
-      </c>
-      <c r="D20">
-        <v>4</v>
-      </c>
-      <c r="E20">
-        <v>3</v>
-      </c>
-      <c r="F20">
-        <v>0.5</v>
-      </c>
-      <c r="G20">
-        <v>7.1000000000000004E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21" t="s">
-        <v>47</v>
-      </c>
-      <c r="C21" t="s">
-        <v>48</v>
-      </c>
-      <c r="D21">
-        <v>11</v>
-      </c>
-      <c r="E21">
-        <v>5</v>
-      </c>
-      <c r="F21">
-        <v>1.38</v>
-      </c>
-      <c r="G21">
-        <v>7.4000000000000003E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" t="s">
-        <v>50</v>
-      </c>
-      <c r="D22">
-        <v>99</v>
-      </c>
-      <c r="E22">
-        <v>21</v>
-      </c>
-      <c r="F22">
+      <c r="H22">
         <v>12.43</v>
       </c>
-      <c r="G22">
+      <c r="I22">
         <v>9.7000000000000003E-3</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="19" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update WGD retention / loss filtering
</commit_message>
<xml_diff>
--- a/HiFi_assemblies/C_amplexicaulis_S_pinnata_comparisons/output/genespace_no_pinnata/WGD_retention_loss_GO.xlsx
+++ b/HiFi_assemblies/C_amplexicaulis_S_pinnata_comparisons/output/genespace_no_pinnata/WGD_retention_loss_GO.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr date1904="1" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jmaloof/git/Davis_Dimensions_Sdiv_Assembly/HiFi_assemblies/C_amplexicaulis_S_pinnata_comparisons/output/genespace_no_pinnata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{E56E9FCE-45E3-764A-9A4E-2E541D845449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CA2D717-DBD1-8540-8807-5F033C9F138D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23780" yWindow="3040" windowWidth="16360" windowHeight="14140" xr2:uid="{8D8973C9-0276-D64F-9CDA-5047CB7ECE61}"/>
+    <workbookView xWindow="23120" yWindow="3420" windowWidth="16360" windowHeight="14140" xr2:uid="{8D8973C9-0276-D64F-9CDA-5047CB7ECE61}"/>
   </bookViews>
   <sheets>
     <sheet name="WGD_retention_loss_GO" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="54">
   <si>
     <t>Category</t>
   </si>
@@ -76,12 +76,6 @@
     <t>S_div. retained</t>
   </si>
   <si>
-    <t>GO:0010073</t>
-  </si>
-  <si>
-    <t>meristem maintenance</t>
-  </si>
-  <si>
     <t>GO:0055085</t>
   </si>
   <si>
@@ -181,13 +175,13 @@
     <t>both single</t>
   </si>
   <si>
-    <t>regulation of DNA-templated transcription</t>
-  </si>
-  <si>
-    <t>chromosome organization involved in meiosis</t>
-  </si>
-  <si>
-    <t>indole-containing compound metabolic process</t>
+    <t>regulation of DNA-templated transcriptio...</t>
+  </si>
+  <si>
+    <t>indole-containing compound metabolic pro...</t>
+  </si>
+  <si>
+    <t>chromosome organization involved in meio...</t>
   </si>
 </sst>
 </file>
@@ -691,12 +685,11 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="11" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1081,10 +1074,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D75D7403-A256-4248-B6EA-CC1A4956221D}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="D2" sqref="D2:I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1100,11 +1093,11 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>50</v>
+      <c r="B1" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>48</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -1113,10 +1106,10 @@
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>3</v>
@@ -1129,68 +1122,68 @@
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="6">
-        <v>2</v>
-      </c>
-      <c r="C2" s="6">
-        <v>2</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="B2" s="5">
+        <v>2</v>
+      </c>
+      <c r="C2" s="5">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" s="3">
+      <c r="E2" t="s">
+        <v>51</v>
+      </c>
+      <c r="F2">
         <v>434</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2">
         <v>355</v>
       </c>
-      <c r="H2" s="3">
-        <v>322.57</v>
-      </c>
-      <c r="I2" s="3">
-        <v>1.9000000000000001E-4</v>
+      <c r="H2">
+        <v>323.18</v>
+      </c>
+      <c r="I2">
+        <v>2.4000000000000001E-4</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="6">
-        <v>2</v>
-      </c>
-      <c r="C3" s="6">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3" t="s">
+      <c r="B3" s="5">
+        <v>2</v>
+      </c>
+      <c r="C3" s="5">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3">
         <v>91</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3">
         <v>80</v>
       </c>
-      <c r="H3" s="3">
-        <v>67.64</v>
-      </c>
-      <c r="I3" s="3">
-        <v>7.2999999999999996E-4</v>
+      <c r="H3">
+        <v>67.760000000000005</v>
+      </c>
+      <c r="I3">
+        <v>7.9000000000000001E-4</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>52</v>
-      </c>
-      <c r="B4" s="7">
+        <v>50</v>
+      </c>
+      <c r="B4" s="6">
         <v>1</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="6">
         <v>1</v>
       </c>
       <c r="D4" t="s">
@@ -1200,26 +1193,26 @@
         <v>10</v>
       </c>
       <c r="F4">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G4">
         <v>37</v>
       </c>
       <c r="H4">
-        <v>19.29</v>
+        <v>19.25</v>
       </c>
       <c r="I4" s="1">
-        <v>1.8E-5</v>
+        <v>1.9000000000000001E-5</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5" s="7">
+        <v>50</v>
+      </c>
+      <c r="B5" s="6">
         <v>1</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6">
         <v>1</v>
       </c>
       <c r="D5" t="s">
@@ -1243,12 +1236,12 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" s="7">
+        <v>50</v>
+      </c>
+      <c r="B6" s="6">
         <v>1</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
@@ -1272,12 +1265,12 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7" s="7">
+        <v>50</v>
+      </c>
+      <c r="B7" s="6">
         <v>1</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6">
         <v>1</v>
       </c>
       <c r="D7" t="s">
@@ -1293,107 +1286,107 @@
         <v>21</v>
       </c>
       <c r="H7">
-        <v>14.11</v>
+        <v>14.14</v>
       </c>
       <c r="I7">
-        <v>7.4000000000000003E-3</v>
+        <v>7.4999999999999997E-3</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="6">
-        <v>2</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D8" s="3" t="s">
+      <c r="B8" s="5">
+        <v>2</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8">
         <v>18</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="3">
-        <v>5</v>
-      </c>
-      <c r="G8" s="3">
+      <c r="G8">
         <v>4</v>
       </c>
-      <c r="H8" s="3">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="I8" s="4">
-        <v>4.6E-5</v>
+      <c r="H8">
+        <v>0.98</v>
+      </c>
+      <c r="I8">
+        <v>2.8999999999999998E-3</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B9" s="6">
-        <v>2</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="3">
-        <v>305</v>
-      </c>
-      <c r="G9" s="3">
-        <v>30</v>
-      </c>
-      <c r="H9" s="3">
-        <v>17.11</v>
-      </c>
-      <c r="I9" s="3">
-        <v>3.0000000000000001E-3</v>
+      <c r="B9" s="5">
+        <v>2</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F9">
+        <v>304</v>
+      </c>
+      <c r="G9">
+        <v>29</v>
+      </c>
+      <c r="H9">
+        <v>16.52</v>
+      </c>
+      <c r="I9">
+        <v>4.1999999999999997E-3</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="6">
-        <v>2</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="A10" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="B10" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C10" s="6">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
         <v>23</v>
       </c>
-      <c r="F10" s="3">
-        <v>18</v>
-      </c>
-      <c r="G10" s="3">
-        <v>4</v>
-      </c>
-      <c r="H10" s="3">
-        <v>1.01</v>
-      </c>
-      <c r="I10" s="3">
-        <v>3.0999999999999999E-3</v>
+      <c r="E10" t="s">
+        <v>24</v>
+      </c>
+      <c r="F10">
+        <v>3</v>
+      </c>
+      <c r="G10">
+        <v>3</v>
+      </c>
+      <c r="H10">
+        <v>0.38</v>
+      </c>
+      <c r="I10">
+        <v>2E-3</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="7">
+        <v>22</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C11" s="6">
         <v>2</v>
       </c>
       <c r="D11" t="s">
@@ -1417,12 +1410,12 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>24</v>
-      </c>
-      <c r="B12" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="7">
+        <v>22</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" s="6">
         <v>2</v>
       </c>
       <c r="D12" t="s">
@@ -1446,12 +1439,12 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C13" s="7">
+        <v>22</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="6">
         <v>2</v>
       </c>
       <c r="D13" t="s">
@@ -1475,12 +1468,12 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C14" s="7">
+        <v>22</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="6">
         <v>2</v>
       </c>
       <c r="D14" t="s">
@@ -1490,26 +1483,26 @@
         <v>32</v>
       </c>
       <c r="F14">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G14">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H14">
-        <v>0.38</v>
+        <v>0.75</v>
       </c>
       <c r="I14">
-        <v>2E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>24</v>
-      </c>
-      <c r="B15" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="7">
+        <v>22</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="6">
         <v>2</v>
       </c>
       <c r="D15" t="s">
@@ -1533,12 +1526,12 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>24</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C16" s="7">
+        <v>22</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C16" s="6">
         <v>2</v>
       </c>
       <c r="D16" t="s">
@@ -1562,19 +1555,19 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="7">
+        <v>22</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="6">
         <v>2</v>
       </c>
       <c r="D17" t="s">
         <v>37</v>
       </c>
       <c r="E17" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="F17">
         <v>6</v>
@@ -1591,48 +1584,48 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>24</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" s="7">
+        <v>22</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="6">
         <v>2</v>
       </c>
       <c r="D18" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" t="s">
         <v>39</v>
       </c>
-      <c r="E18" t="s">
-        <v>55</v>
-      </c>
       <c r="F18">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G18">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H18">
-        <v>0.75</v>
+        <v>0.5</v>
       </c>
       <c r="I18">
-        <v>3.0000000000000001E-3</v>
+        <v>7.1999999999999998E-3</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="7">
+        <v>22</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="6">
         <v>2</v>
       </c>
       <c r="D19" t="s">
         <v>40</v>
       </c>
       <c r="E19" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="F19">
         <v>4</v>
@@ -1644,46 +1637,46 @@
         <v>0.5</v>
       </c>
       <c r="I19">
-        <v>7.1000000000000004E-3</v>
+        <v>7.1999999999999998E-3</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="7">
+        <v>22</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="6">
         <v>2</v>
       </c>
       <c r="D20" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" t="s">
         <v>42</v>
       </c>
-      <c r="E20" t="s">
-        <v>54</v>
-      </c>
       <c r="F20">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="G20">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H20">
-        <v>0.5</v>
+        <v>1.38</v>
       </c>
       <c r="I20">
-        <v>7.1000000000000004E-3</v>
+        <v>7.4000000000000003E-3</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>24</v>
-      </c>
-      <c r="B21" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="7">
+        <v>22</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C21" s="6">
         <v>2</v>
       </c>
       <c r="D21" t="s">
@@ -1693,45 +1686,16 @@
         <v>44</v>
       </c>
       <c r="F21">
-        <v>11</v>
+        <v>99</v>
       </c>
       <c r="G21">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="H21">
-        <v>1.38</v>
+        <v>12.45</v>
       </c>
       <c r="I21">
-        <v>7.4000000000000003E-3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="7">
-        <v>2</v>
-      </c>
-      <c r="D22" t="s">
-        <v>45</v>
-      </c>
-      <c r="E22" t="s">
-        <v>46</v>
-      </c>
-      <c r="F22">
-        <v>99</v>
-      </c>
-      <c r="G22">
-        <v>21</v>
-      </c>
-      <c r="H22">
-        <v>12.43</v>
-      </c>
-      <c r="I22">
-        <v>9.7000000000000003E-3</v>
+        <v>9.9000000000000008E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>